<commit_message>
modified:   list.xlsx 	modified:   out.csv 	modified:   sentiment_analysis.ipynb
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
   <si>
     <t>I spent the whole day in my head</t>
   </si>
@@ -24,15 +24,6 @@
     <t>Do a little spring cleanin'</t>
   </si>
   <si>
-    <t>I'm always too busy dreamin'</t>
-  </si>
-  <si>
-    <t>Well, maybe I should wake up instead</t>
-  </si>
-  <si>
-    <t>A lot of things I regret, but I just say I forget</t>
-  </si>
-  <si>
     <t>Why can't it just be easy?</t>
   </si>
   <si>
@@ -166,13 +157,31 @@
   </si>
   <si>
     <t>At least it don't gotta be no more</t>
+  </si>
+  <si>
+    <t>No more, no more, no more, no more</t>
+  </si>
+  <si>
+    <t>Hey, hey</t>
+  </si>
+  <si>
+    <t>Mm, hey, mm, mm, mm</t>
+  </si>
+  <si>
+    <t>I'm always too busy dreamin'</t>
+  </si>
+  <si>
+    <t>Well, maybe I should wake up instead</t>
+  </si>
+  <si>
+    <t>A lot of things I regret, but I just say I forget</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +193,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -210,9 +225,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -515,340 +531,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A58"/>
+  <dimension ref="A1:A62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>44</v>
+      <c r="A51" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>45</v>
+      <c r="A52" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>45</v>
+      <c r="A53" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>43</v>
+      <c r="A54" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://genius.com/18808644/Mac-miller-good-news/I-spent-the-whole-day-in-my-head-do-a-little-spring-cleanin"/>
-    <hyperlink ref="A2" r:id="rId2" display="https://genius.com/18808644/Mac-miller-good-news/I-spent-the-whole-day-in-my-head-do-a-little-spring-cleanin"/>
-    <hyperlink ref="A9" r:id="rId3" display="https://genius.com/19106929/Mac-miller-good-news/When-youre-high-but-youre-underneath-the-ceilin"/>
-    <hyperlink ref="A10" r:id="rId4" display="https://genius.com/18806948/Mac-miller-good-news/Got-the-cards-in-my-hand-i-hate-dealin-yeah"/>
-    <hyperlink ref="A15" r:id="rId5" display="https://genius.com/20876442/Mac-miller-good-news/There-aint-a-better-time-than-today-well-maybe-ill-lay-down-for-a-little-yeah-instead-of-always-tryin-to-figure-everything-out"/>
-    <hyperlink ref="A16" r:id="rId6" display="https://genius.com/20876442/Mac-miller-good-news/There-aint-a-better-time-than-today-well-maybe-ill-lay-down-for-a-little-yeah-instead-of-always-tryin-to-figure-everything-out"/>
-    <hyperlink ref="A17" r:id="rId7" display="https://genius.com/20876442/Mac-miller-good-news/There-aint-a-better-time-than-today-well-maybe-ill-lay-down-for-a-little-yeah-instead-of-always-tryin-to-figure-everything-out"/>
-    <hyperlink ref="A18" r:id="rId8" display="https://genius.com/20876387/Mac-miller-good-news/And-all-i-do-is-say-sorry-half-the-time-i-dont-even-know-what-im-sayin-it-about"/>
-    <hyperlink ref="A19" r:id="rId9" display="https://genius.com/20876387/Mac-miller-good-news/And-all-i-do-is-say-sorry-half-the-time-i-dont-even-know-what-im-sayin-it-about"/>
-    <hyperlink ref="A22" r:id="rId10" display="https://genius.com/30224757/Mac-miller-good-news/No-they-dont-like-it-when-im-down-but-when-im-flyin-oh-it-make-em-so-uncomfortable-so-different-whats-the-difference"/>
-    <hyperlink ref="A23" r:id="rId11" display="https://genius.com/30224757/Mac-miller-good-news/No-they-dont-like-it-when-im-down-but-when-im-flyin-oh-it-make-em-so-uncomfortable-so-different-whats-the-difference"/>
-    <hyperlink ref="A24" r:id="rId12" display="https://genius.com/30224757/Mac-miller-good-news/No-they-dont-like-it-when-im-down-but-when-im-flyin-oh-it-make-em-so-uncomfortable-so-different-whats-the-difference"/>
-    <hyperlink ref="A25" r:id="rId13" display="https://genius.com/30224757/Mac-miller-good-news/No-they-dont-like-it-when-im-down-but-when-im-flyin-oh-it-make-em-so-uncomfortable-so-different-whats-the-difference"/>
-    <hyperlink ref="A28" r:id="rId14" display="https://genius.com/20876427/Mac-miller-good-news/Im-runnin-out-of-gas-hardly-anything-left-hope-i-make-it-home-from-work-well-so-tired-of-bein-so-tired"/>
-    <hyperlink ref="A29" r:id="rId15" display="https://genius.com/20876427/Mac-miller-good-news/Im-runnin-out-of-gas-hardly-anything-left-hope-i-make-it-home-from-work-well-so-tired-of-bein-so-tired"/>
-    <hyperlink ref="A30" r:id="rId16" display="https://genius.com/20876427/Mac-miller-good-news/Im-runnin-out-of-gas-hardly-anything-left-hope-i-make-it-home-from-work-well-so-tired-of-bein-so-tired"/>
-    <hyperlink ref="A31" r:id="rId17" display="https://genius.com/30575745/Mac-miller-good-news/Why-i-gotta-build-somethin-beautiful-just-to-go-set-it-on-fire"/>
-    <hyperlink ref="A32" r:id="rId18" display="https://genius.com/20516654/Mac-miller-good-news/Im-no-liar-but-sometimes-the-truth-dont-sound-like-the-truth-maybe-cause-it-aint-i-just-love-the-way-it-sound-when-i-say-it"/>
-    <hyperlink ref="A33" r:id="rId19" display="https://genius.com/20516654/Mac-miller-good-news/Im-no-liar-but-sometimes-the-truth-dont-sound-like-the-truth-maybe-cause-it-aint-i-just-love-the-way-it-sound-when-i-say-it"/>
-    <hyperlink ref="A34" r:id="rId20" display="https://genius.com/20516654/Mac-miller-good-news/Im-no-liar-but-sometimes-the-truth-dont-sound-like-the-truth-maybe-cause-it-aint-i-just-love-the-way-it-sound-when-i-say-it"/>
-    <hyperlink ref="A35" r:id="rId21" display="https://genius.com/20516654/Mac-miller-good-news/Im-no-liar-but-sometimes-the-truth-dont-sound-like-the-truth-maybe-cause-it-aint-i-just-love-the-way-it-sound-when-i-say-it"/>
-    <hyperlink ref="A38" r:id="rId22" display="https://genius.com/20516674/Mac-miller-good-news/Wake-up-to-the-moon-havent-seen-the-sun-in-a-while-but-i-heard-that-the-skys-still-blue-yeah"/>
-    <hyperlink ref="A39" r:id="rId23" display="https://genius.com/20516674/Mac-miller-good-news/Wake-up-to-the-moon-havent-seen-the-sun-in-a-while-but-i-heard-that-the-skys-still-blue-yeah"/>
-    <hyperlink ref="A40" r:id="rId24" display="https://genius.com/18864814/Mac-miller-good-news/I-heard-they-dont-talk-about-me-too-much-no-more-and-thats-the-problem-with-a-closed-door"/>
-    <hyperlink ref="A41" r:id="rId25" display="https://genius.com/18864814/Mac-miller-good-news/I-heard-they-dont-talk-about-me-too-much-no-more-and-thats-the-problem-with-a-closed-door"/>
-    <hyperlink ref="A48" r:id="rId26" display="https://genius.com/20516690/Mac-miller-good-news/Theres-a-whole-lot-more-for-me-waitin-on-the-other-side-im-always-wonderin-if-it-feel-like-summer"/>
-    <hyperlink ref="A49" r:id="rId27" display="https://genius.com/20516690/Mac-miller-good-news/Theres-a-whole-lot-more-for-me-waitin-on-the-other-side-im-always-wonderin-if-it-feel-like-summer"/>
-    <hyperlink ref="A50" r:id="rId28" display="https://genius.com/18882658/Mac-miller-good-news/I-know-maybe-im-too-late-i-could-make-it-there-some-other-time"/>
-    <hyperlink ref="A55" r:id="rId29" display="https://genius.com/21973450/Mac-miller-good-news/Then-ill-finally-discover-that-it-aint-that-bad-aint-so-bad-well-it-aint-that-bad-mm-at-least-it-dont-gotta-be-no-more"/>
-    <hyperlink ref="A56" r:id="rId30" display="https://genius.com/21973450/Mac-miller-good-news/Then-ill-finally-discover-that-it-aint-that-bad-aint-so-bad-well-it-aint-that-bad-mm-at-least-it-dont-gotta-be-no-more"/>
-    <hyperlink ref="A57" r:id="rId31" display="https://genius.com/21973450/Mac-miller-good-news/Then-ill-finally-discover-that-it-aint-that-bad-aint-so-bad-well-it-aint-that-bad-mm-at-least-it-dont-gotta-be-no-more"/>
-    <hyperlink ref="A58" r:id="rId32" display="https://genius.com/21973450/Mac-miller-good-news/Then-ill-finally-discover-that-it-aint-that-bad-aint-so-bad-well-it-aint-that-bad-mm-at-least-it-dont-gotta-be-no-more"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>